<commit_message>
Updates GBF Indicator A.2 Excel template.
Updates the GBF Indicator A.2 Excel template with the latest version.
</commit_message>
<xml_diff>
--- a/public/excel-templates/GBF-INDICATOR-A.2.xlsx
+++ b/public/excel-templates/GBF-INDICATOR-A.2.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitednations-my.sharepoint.com/personal/kieran_mooney_un_org/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{884C53B1-6844-4DDF-A6B5-937E628B2FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B125F37-551E-49FD-8816-F8258611764C}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{BAF05321-588B-4D30-9905-263CFA046011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95269A53-01C7-4B4E-9CEF-6B6C0F1C357E}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Lups1S0s81onf963Dew7RuymzSvbho8ThFqMIhcQaTQT6F9WhssamukkcEEVVBfSoZ335eQX75fDDSuSKebfig==" workbookSaltValue="/Ar7ECGItDTTKR3BKDn/hg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A2" sheetId="8" r:id="rId1"/>
@@ -1070,24 +1070,24 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="30" style="18" customWidth="1"/>
     <col min="6" max="6" width="11" style="18" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" style="18"/>
-    <col min="9" max="9" width="24.1796875" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" style="2"/>
+    <col min="7" max="7" width="9.85546875" style="18" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="18"/>
+    <col min="9" max="9" width="24.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -1137,7 +1137,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="H3" s="17"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="H7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -1281,523 +1281,523 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="3"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="3"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="3"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="3"/>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="3"/>
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3"/>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="3"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="3"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="3"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="3"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="3"/>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="3"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="3"/>
       <c r="E38" s="15"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="3"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="3"/>
       <c r="E40" s="15"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="3"/>
       <c r="E41" s="15"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="3"/>
       <c r="E42" s="15"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="3"/>
       <c r="E43" s="15"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="3"/>
       <c r="E44" s="15"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="3"/>
       <c r="E45" s="15"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="3"/>
       <c r="E46" s="15"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="3"/>
       <c r="E47" s="15"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="3"/>
       <c r="E48" s="15"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="3"/>
       <c r="E49" s="15"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="3"/>
       <c r="E50" s="15"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="3"/>
       <c r="E51" s="15"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="3"/>
       <c r="E52" s="15"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
       <c r="E53" s="15"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="3"/>
       <c r="E54" s="15"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="3"/>
       <c r="E55" s="15"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="3"/>
       <c r="E56" s="15"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="3"/>
       <c r="E57" s="15"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="3"/>
       <c r="E58" s="15"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="3"/>
       <c r="E59" s="15"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="3"/>
       <c r="E60" s="15"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="3"/>
       <c r="E61" s="15"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="3"/>
       <c r="E62" s="15"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="3"/>
       <c r="E63" s="15"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="3"/>
       <c r="E64" s="15"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="3"/>
       <c r="E65" s="15"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="3"/>
       <c r="E66" s="15"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="3"/>
       <c r="E67" s="15"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="3"/>
       <c r="E68" s="15"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="3"/>
       <c r="E69" s="15"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="3"/>
       <c r="E70" s="15"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="3"/>
       <c r="E71" s="15"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="3"/>
       <c r="E72" s="15"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="3"/>
       <c r="E73" s="15"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="3"/>
       <c r="E74" s="15"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="3"/>
       <c r="E75" s="15"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="3"/>
       <c r="E76" s="15"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="3"/>
       <c r="E77" s="15"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="3"/>
       <c r="E78" s="15"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="3"/>
       <c r="E79" s="15"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="3"/>
       <c r="E80" s="15"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="3"/>
       <c r="E81" s="15"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="3"/>
       <c r="E82" s="15"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="3"/>
       <c r="E83" s="15"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="3"/>
       <c r="E84" s="15"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="3"/>
       <c r="E85" s="15"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="3"/>
       <c r="E86" s="15"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="3"/>
       <c r="E87" s="15"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="3"/>
       <c r="E88" s="15"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="3"/>
       <c r="E89" s="15"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="3"/>
       <c r="E90" s="15"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="3"/>
       <c r="E91" s="15"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="3"/>
       <c r="E92" s="15"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="3"/>
       <c r="E93" s="15"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="3"/>
       <c r="E94" s="15"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="3" t="str">
-        <f t="shared" ref="D67:D100" si="2">IF(C95="","",IF(C95="Yes","[Please select the disaggregation type from the drop down list]",IF(C95="No","Not applicable")))</f>
+        <f t="shared" ref="D95:D100" si="2">IF(C95="","",IF(C95="Yes","[Please select the disaggregation type from the drop down list]",IF(C95="No","Not applicable")))</f>
         <v/>
       </c>
       <c r="E95" s="15" t="str">
-        <f t="shared" ref="E67:E100" si="3">IF(D95="","",IF(D95="Not applicable","Not applicable",IF(D95="Biome - Global Ecosystem Typology level 2","[Please select the relevant category from the drop down list]",IF(D95="Ecosystem Functional Group - Global Ecosystem typology level 3","[Please select the relevant category from the drop down list]",IF(D95="Indigenous and traditional territories","[Please describe]",IF(D95="Protected areas or other effective area-based conservation measures","[Please describe]",IF(D95="Restoration activity - PRAIS action type","[Please select the relevant category from the drop down list]",IF(D95="Other","[Please describe]"))))))))</f>
+        <f t="shared" ref="E95:E100" si="3">IF(D95="","",IF(D95="Not applicable","Not applicable",IF(D95="Biome - Global Ecosystem Typology level 2","[Please select the relevant category from the drop down list]",IF(D95="Ecosystem Functional Group - Global Ecosystem typology level 3","[Please select the relevant category from the drop down list]",IF(D95="Indigenous and traditional territories","[Please describe]",IF(D95="Protected areas or other effective area-based conservation measures","[Please describe]",IF(D95="Restoration activity - PRAIS action type","[Please select the relevant category from the drop down list]",IF(D95="Other","[Please describe]"))))))))</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="3" t="str">
@@ -1809,7 +1809,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="3" t="str">
@@ -1821,7 +1821,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="3" t="str">
@@ -1833,7 +1833,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="3" t="str">
@@ -1845,7 +1845,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="3" t="str">
@@ -1858,33 +1858,27 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0"/>
+  <sheetProtection insertRows="0"/>
   <dataConsolidate/>
-  <dataValidations count="2">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C100" xr:uid="{A2A3EBD1-701E-4AA5-B6D2-8B8742FA50DC}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{F544BA18-FB28-49F2-A99E-2F7A4E942AEB}">
       <formula1>"Yes, No, - "</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E11:E100" xr:uid="{ADCED1F8-2D1D-46BF-97C2-23AEC6E95569}">
+      <formula1>_xlfn.XLOOKUP(D11,#REF!,#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D11:D100" xr:uid="{CB4D3523-F8AF-4D7E-BCC3-226F3824A2EF}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{ADCED1F8-2D1D-46BF-97C2-23AEC6E95569}">
-          <x14:formula1>
-            <xm:f>_xlfn.XLOOKUP(D11,#REF!,#REF!)</xm:f>
-          </x14:formula1>
-          <xm:sqref>E11:E100</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{CB4D3523-F8AF-4D7E-BCC3-226F3824A2EF}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D11:D100</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{FBA5F84C-7222-46B3-87C5-0309D57379B9}">
           <x14:formula1>
             <xm:f>_xlfn.XLOOKUP(D2,'A.2 Category information'!$A$1:$E$1,'A.2 Category information'!$A$2:$E$96)</xm:f>
@@ -1909,17 +1903,17 @@
   <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>123</v>
       </c>
@@ -1936,7 +1930,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1949,7 +1943,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1962,7 +1956,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1973,7 +1967,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1984,7 +1978,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1995,7 +1989,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -2006,7 +2000,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -2017,7 +2011,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -2028,7 +2022,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2039,7 +2033,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -2050,7 +2044,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
@@ -2061,7 +2055,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -2072,7 +2066,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -2083,7 +2077,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -2094,7 +2088,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
@@ -2105,7 +2099,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
@@ -2116,7 +2110,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
@@ -2127,7 +2121,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
@@ -2138,7 +2132,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
@@ -2149,7 +2143,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -2160,7 +2154,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
@@ -2171,7 +2165,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
@@ -2182,7 +2176,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>30</v>
       </c>
@@ -2193,7 +2187,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
@@ -2204,7 +2198,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
@@ -2215,7 +2209,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="11" t="s">
         <v>57</v>
@@ -2224,7 +2218,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="10" t="s">
         <v>58</v>
@@ -2233,7 +2227,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="11" t="s">
         <v>59</v>
@@ -2242,7 +2236,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="10" t="s">
         <v>60</v>
@@ -2251,7 +2245,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="12" t="s">
         <v>132</v>
@@ -2260,7 +2254,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="13" t="s">
         <v>133</v>
@@ -2269,7 +2263,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="12" t="s">
         <v>134</v>
@@ -2278,7 +2272,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="13" t="s">
         <v>135</v>
@@ -2287,7 +2281,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="11" t="s">
         <v>61</v>
@@ -2296,7 +2290,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="10" t="s">
         <v>62</v>
@@ -2305,7 +2299,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="11" t="s">
         <v>63</v>
@@ -2314,7 +2308,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="13" t="s">
         <v>136</v>
@@ -2323,7 +2317,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="11" t="s">
         <v>64</v>
@@ -2332,7 +2326,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="10" t="s">
         <v>65</v>
@@ -2341,7 +2335,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="12" t="s">
         <v>137</v>
@@ -2350,7 +2344,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="13" t="s">
         <v>138</v>
@@ -2359,7 +2353,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="11" t="s">
         <v>66</v>
@@ -2368,7 +2362,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="10" t="s">
         <v>67</v>
@@ -2377,7 +2371,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="11" t="s">
         <v>68</v>
@@ -2386,7 +2380,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="10" t="s">
         <v>69</v>
@@ -2395,7 +2389,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="11" t="s">
         <v>70</v>
@@ -2404,7 +2398,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="10" t="s">
         <v>71</v>
@@ -2413,7 +2407,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="11" t="s">
         <v>72</v>
@@ -2422,7 +2416,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="10" t="s">
         <v>73</v>
@@ -2431,7 +2425,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="11" t="s">
         <v>74</v>
@@ -2440,7 +2434,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="10" t="s">
         <v>75</v>
@@ -2449,7 +2443,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="12" t="s">
         <v>139</v>
@@ -2458,7 +2452,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="13" t="s">
         <v>140</v>
@@ -2467,7 +2461,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="11" t="s">
         <v>76</v>
@@ -2476,7 +2470,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="13" t="s">
         <v>141</v>
@@ -2485,7 +2479,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="12" t="s">
         <v>142</v>
@@ -2494,7 +2488,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="13" t="s">
         <v>143</v>
@@ -2503,7 +2497,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="12" t="s">
         <v>144</v>
@@ -2512,7 +2506,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="10" t="s">
         <v>77</v>
@@ -2521,7 +2515,7 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="11" t="s">
         <v>78</v>
@@ -2530,7 +2524,7 @@
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="10" t="s">
         <v>79</v>
@@ -2539,7 +2533,7 @@
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="11" t="s">
         <v>80</v>
@@ -2548,7 +2542,7 @@
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="10" t="s">
         <v>81</v>
@@ -2557,7 +2551,7 @@
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="11" t="s">
         <v>82</v>
@@ -2566,7 +2560,7 @@
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="10" t="s">
         <v>83</v>
@@ -2575,7 +2569,7 @@
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="11" t="s">
         <v>84</v>
@@ -2584,7 +2578,7 @@
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="10" t="s">
         <v>85</v>
@@ -2593,7 +2587,7 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="11" t="s">
         <v>86</v>
@@ -2602,7 +2596,7 @@
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="13" t="s">
         <v>145</v>
@@ -2611,7 +2605,7 @@
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="12" t="s">
         <v>146</v>
@@ -2620,7 +2614,7 @@
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="13" t="s">
         <v>147</v>
@@ -2629,7 +2623,7 @@
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="12" t="s">
         <v>148</v>
@@ -2638,7 +2632,7 @@
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="13" t="s">
         <v>149</v>
@@ -2647,7 +2641,7 @@
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="11" t="s">
         <v>87</v>
@@ -2656,7 +2650,7 @@
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="10" t="s">
         <v>88</v>
@@ -2665,7 +2659,7 @@
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="11" t="s">
         <v>89</v>
@@ -2674,7 +2668,7 @@
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="10" t="s">
         <v>90</v>
@@ -2683,7 +2677,7 @@
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="11" t="s">
         <v>91</v>
@@ -2692,7 +2686,7 @@
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="10" t="s">
         <v>92</v>
@@ -2701,7 +2695,7 @@
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="11" t="s">
         <v>93</v>
@@ -2710,7 +2704,7 @@
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="10" t="s">
         <v>94</v>
@@ -2719,7 +2713,7 @@
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="11" t="s">
         <v>95</v>
@@ -2728,7 +2722,7 @@
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="10" t="s">
         <v>96</v>
@@ -2737,7 +2731,7 @@
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="11" t="s">
         <v>97</v>
@@ -2746,7 +2740,7 @@
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="10" t="s">
         <v>98</v>
@@ -2755,7 +2749,7 @@
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="11" t="s">
         <v>99</v>
@@ -2764,7 +2758,7 @@
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="10" t="s">
         <v>100</v>
@@ -2773,7 +2767,7 @@
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="11" t="s">
         <v>101</v>
@@ -2782,7 +2776,7 @@
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="10" t="s">
         <v>102</v>
@@ -2791,7 +2785,7 @@
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="11" t="s">
         <v>103</v>
@@ -2800,7 +2794,7 @@
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="10" t="s">
         <v>104</v>
@@ -2809,7 +2803,7 @@
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="11" t="s">
         <v>105</v>
@@ -2818,7 +2812,7 @@
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="10" t="s">
         <v>106</v>
@@ -2827,7 +2821,7 @@
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="11" t="s">
         <v>107</v>
@@ -2836,7 +2830,7 @@
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="10" t="s">
         <v>108</v>
@@ -2845,7 +2839,7 @@
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="11" t="s">
         <v>109</v>
@@ -2854,7 +2848,7 @@
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="10" t="s">
         <v>110</v>
@@ -2863,7 +2857,7 @@
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="11" t="s">
         <v>111</v>
@@ -2872,7 +2866,7 @@
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="B100" s="13" t="s">
         <v>150</v>
@@ -2881,7 +2875,7 @@
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="12" t="s">
         <v>151</v>
@@ -2890,7 +2884,7 @@
       <c r="D101" s="6"/>
       <c r="E101" s="6"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
       <c r="B102" s="10" t="s">
         <v>112</v>
@@ -2899,7 +2893,7 @@
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="11" t="s">
         <v>113</v>
@@ -2908,7 +2902,7 @@
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="10" t="s">
         <v>114</v>
@@ -2917,7 +2911,7 @@
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="11" t="s">
         <v>115</v>
@@ -2926,7 +2920,7 @@
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
       <c r="B106" s="10" t="s">
         <v>116</v>
@@ -2935,7 +2929,7 @@
       <c r="D106" s="6"/>
       <c r="E106" s="6"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="11" t="s">
         <v>117</v>
@@ -2944,7 +2938,7 @@
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="13" t="s">
         <v>152</v>
@@ -2953,7 +2947,7 @@
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="11" t="s">
         <v>118</v>
@@ -2962,7 +2956,7 @@
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
       <c r="B110" s="10" t="s">
         <v>119</v>
@@ -2971,7 +2965,7 @@
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
       <c r="B111" s="9" t="s">
         <v>120</v>
@@ -2990,15 +2984,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003082C08FD3D0614AAB94B75C024070A7" ma:contentTypeVersion="29" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a4b61487ffa532d49c6719891dd0d2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="82302deb-32b0-442b-bedc-ba64a9aa8ccd" xmlns:ns3="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cea40d1c5f6ee0e5ae997cf8704aff88" ns2:_="" ns3:_="">
     <xsd:import namespace="82302deb-32b0-442b-bedc-ba64a9aa8ccd"/>
@@ -3287,6 +3272,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3306,14 +3300,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{675DE784-F3DF-4BF9-9432-B8FB7941C39F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B39BBA2A-0161-425D-935A-F961630DCAA3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3328,6 +3314,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{675DE784-F3DF-4BF9-9432-B8FB7941C39F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Misc improvements to NR7 section III & IV (#210)
</commit_message>
<xml_diff>
--- a/public/excel-templates/GBF-INDICATOR-A.2.xlsx
+++ b/public/excel-templates/GBF-INDICATOR-A.2.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitednations-my.sharepoint.com/personal/kieran_mooney_un_org/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{884C53B1-6844-4DDF-A6B5-937E628B2FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B125F37-551E-49FD-8816-F8258611764C}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{BAF05321-588B-4D30-9905-263CFA046011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95269A53-01C7-4B4E-9CEF-6B6C0F1C357E}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Lups1S0s81onf963Dew7RuymzSvbho8ThFqMIhcQaTQT6F9WhssamukkcEEVVBfSoZ335eQX75fDDSuSKebfig==" workbookSaltValue="/Ar7ECGItDTTKR3BKDn/hg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A2" sheetId="8" r:id="rId1"/>
@@ -1070,24 +1070,24 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="30" style="18" customWidth="1"/>
     <col min="6" max="6" width="11" style="18" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" style="18"/>
-    <col min="9" max="9" width="24.1796875" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" style="2"/>
+    <col min="7" max="7" width="9.85546875" style="18" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="18"/>
+    <col min="9" max="9" width="24.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -1137,7 +1137,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="H3" s="17"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="H4" s="19"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="H7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -1281,523 +1281,523 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="3"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="3"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="3"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="3"/>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="3"/>
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3"/>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="3"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="3"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="3"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="3"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="3"/>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="3"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="3"/>
       <c r="E38" s="15"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="3"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="3"/>
       <c r="E40" s="15"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="3"/>
       <c r="E41" s="15"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="3"/>
       <c r="E42" s="15"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="3"/>
       <c r="E43" s="15"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="3"/>
       <c r="E44" s="15"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="3"/>
       <c r="E45" s="15"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="3"/>
       <c r="E46" s="15"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="3"/>
       <c r="E47" s="15"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="3"/>
       <c r="E48" s="15"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="3"/>
       <c r="E49" s="15"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="3"/>
       <c r="E50" s="15"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="3"/>
       <c r="E51" s="15"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="3"/>
       <c r="E52" s="15"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
       <c r="E53" s="15"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="3"/>
       <c r="E54" s="15"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="3"/>
       <c r="E55" s="15"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="3"/>
       <c r="E56" s="15"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="3"/>
       <c r="E57" s="15"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="3"/>
       <c r="E58" s="15"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="3"/>
       <c r="E59" s="15"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="3"/>
       <c r="E60" s="15"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="3"/>
       <c r="E61" s="15"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="3"/>
       <c r="E62" s="15"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="3"/>
       <c r="E63" s="15"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="3"/>
       <c r="E64" s="15"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="3"/>
       <c r="E65" s="15"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="3"/>
       <c r="E66" s="15"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="3"/>
       <c r="E67" s="15"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="3"/>
       <c r="E68" s="15"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="3"/>
       <c r="E69" s="15"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="3"/>
       <c r="E70" s="15"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="3"/>
       <c r="E71" s="15"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="3"/>
       <c r="E72" s="15"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="3"/>
       <c r="E73" s="15"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="3"/>
       <c r="E74" s="15"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="3"/>
       <c r="E75" s="15"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="3"/>
       <c r="E76" s="15"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="3"/>
       <c r="E77" s="15"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="3"/>
       <c r="E78" s="15"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="3"/>
       <c r="E79" s="15"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="3"/>
       <c r="E80" s="15"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="3"/>
       <c r="E81" s="15"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="3"/>
       <c r="E82" s="15"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="3"/>
       <c r="E83" s="15"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="3"/>
       <c r="E84" s="15"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="3"/>
       <c r="E85" s="15"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="3"/>
       <c r="E86" s="15"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="3"/>
       <c r="E87" s="15"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="3"/>
       <c r="E88" s="15"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="3"/>
       <c r="E89" s="15"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="3"/>
       <c r="E90" s="15"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="3"/>
       <c r="E91" s="15"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="3"/>
       <c r="E92" s="15"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="3"/>
       <c r="E93" s="15"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="3"/>
       <c r="E94" s="15"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="3" t="str">
-        <f t="shared" ref="D67:D100" si="2">IF(C95="","",IF(C95="Yes","[Please select the disaggregation type from the drop down list]",IF(C95="No","Not applicable")))</f>
+        <f t="shared" ref="D95:D100" si="2">IF(C95="","",IF(C95="Yes","[Please select the disaggregation type from the drop down list]",IF(C95="No","Not applicable")))</f>
         <v/>
       </c>
       <c r="E95" s="15" t="str">
-        <f t="shared" ref="E67:E100" si="3">IF(D95="","",IF(D95="Not applicable","Not applicable",IF(D95="Biome - Global Ecosystem Typology level 2","[Please select the relevant category from the drop down list]",IF(D95="Ecosystem Functional Group - Global Ecosystem typology level 3","[Please select the relevant category from the drop down list]",IF(D95="Indigenous and traditional territories","[Please describe]",IF(D95="Protected areas or other effective area-based conservation measures","[Please describe]",IF(D95="Restoration activity - PRAIS action type","[Please select the relevant category from the drop down list]",IF(D95="Other","[Please describe]"))))))))</f>
+        <f t="shared" ref="E95:E100" si="3">IF(D95="","",IF(D95="Not applicable","Not applicable",IF(D95="Biome - Global Ecosystem Typology level 2","[Please select the relevant category from the drop down list]",IF(D95="Ecosystem Functional Group - Global Ecosystem typology level 3","[Please select the relevant category from the drop down list]",IF(D95="Indigenous and traditional territories","[Please describe]",IF(D95="Protected areas or other effective area-based conservation measures","[Please describe]",IF(D95="Restoration activity - PRAIS action type","[Please select the relevant category from the drop down list]",IF(D95="Other","[Please describe]"))))))))</f>
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="3" t="str">
@@ -1809,7 +1809,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="3" t="str">
@@ -1821,7 +1821,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="3" t="str">
@@ -1833,7 +1833,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="3" t="str">
@@ -1845,7 +1845,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="3" t="str">
@@ -1858,33 +1858,27 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0"/>
+  <sheetProtection insertRows="0"/>
   <dataConsolidate/>
-  <dataValidations count="2">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C100" xr:uid="{A2A3EBD1-701E-4AA5-B6D2-8B8742FA50DC}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{F544BA18-FB28-49F2-A99E-2F7A4E942AEB}">
       <formula1>"Yes, No, - "</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E11:E100" xr:uid="{ADCED1F8-2D1D-46BF-97C2-23AEC6E95569}">
+      <formula1>_xlfn.XLOOKUP(D11,#REF!,#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D11:D100" xr:uid="{CB4D3523-F8AF-4D7E-BCC3-226F3824A2EF}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{ADCED1F8-2D1D-46BF-97C2-23AEC6E95569}">
-          <x14:formula1>
-            <xm:f>_xlfn.XLOOKUP(D11,#REF!,#REF!)</xm:f>
-          </x14:formula1>
-          <xm:sqref>E11:E100</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{CB4D3523-F8AF-4D7E-BCC3-226F3824A2EF}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D11:D100</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{FBA5F84C-7222-46B3-87C5-0309D57379B9}">
           <x14:formula1>
             <xm:f>_xlfn.XLOOKUP(D2,'A.2 Category information'!$A$1:$E$1,'A.2 Category information'!$A$2:$E$96)</xm:f>
@@ -1909,17 +1903,17 @@
   <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>123</v>
       </c>
@@ -1936,7 +1930,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1949,7 +1943,7 @@
       </c>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1962,7 +1956,7 @@
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1973,7 +1967,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1984,7 +1978,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1995,7 +1989,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
@@ -2006,7 +2000,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -2017,7 +2011,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
@@ -2028,7 +2022,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2039,7 +2033,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -2050,7 +2044,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
@@ -2061,7 +2055,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -2072,7 +2066,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -2083,7 +2077,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -2094,7 +2088,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
@@ -2105,7 +2099,7 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
@@ -2116,7 +2110,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
@@ -2127,7 +2121,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
@@ -2138,7 +2132,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
@@ -2149,7 +2143,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -2160,7 +2154,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
@@ -2171,7 +2165,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
@@ -2182,7 +2176,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>30</v>
       </c>
@@ -2193,7 +2187,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>31</v>
       </c>
@@ -2204,7 +2198,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
@@ -2215,7 +2209,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="11" t="s">
         <v>57</v>
@@ -2224,7 +2218,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="10" t="s">
         <v>58</v>
@@ -2233,7 +2227,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="11" t="s">
         <v>59</v>
@@ -2242,7 +2236,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="10" t="s">
         <v>60</v>
@@ -2251,7 +2245,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="12" t="s">
         <v>132</v>
@@ -2260,7 +2254,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="13" t="s">
         <v>133</v>
@@ -2269,7 +2263,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="12" t="s">
         <v>134</v>
@@ -2278,7 +2272,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="13" t="s">
         <v>135</v>
@@ -2287,7 +2281,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="11" t="s">
         <v>61</v>
@@ -2296,7 +2290,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="10" t="s">
         <v>62</v>
@@ -2305,7 +2299,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="11" t="s">
         <v>63</v>
@@ -2314,7 +2308,7 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="13" t="s">
         <v>136</v>
@@ -2323,7 +2317,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="11" t="s">
         <v>64</v>
@@ -2332,7 +2326,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="10" t="s">
         <v>65</v>
@@ -2341,7 +2335,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="12" t="s">
         <v>137</v>
@@ -2350,7 +2344,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="13" t="s">
         <v>138</v>
@@ -2359,7 +2353,7 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="11" t="s">
         <v>66</v>
@@ -2368,7 +2362,7 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="10" t="s">
         <v>67</v>
@@ -2377,7 +2371,7 @@
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="11" t="s">
         <v>68</v>
@@ -2386,7 +2380,7 @@
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="10" t="s">
         <v>69</v>
@@ -2395,7 +2389,7 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="11" t="s">
         <v>70</v>
@@ -2404,7 +2398,7 @@
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="10" t="s">
         <v>71</v>
@@ -2413,7 +2407,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="11" t="s">
         <v>72</v>
@@ -2422,7 +2416,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="10" t="s">
         <v>73</v>
@@ -2431,7 +2425,7 @@
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="11" t="s">
         <v>74</v>
@@ -2440,7 +2434,7 @@
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="10" t="s">
         <v>75</v>
@@ -2449,7 +2443,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="12" t="s">
         <v>139</v>
@@ -2458,7 +2452,7 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="13" t="s">
         <v>140</v>
@@ -2467,7 +2461,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="11" t="s">
         <v>76</v>
@@ -2476,7 +2470,7 @@
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="13" t="s">
         <v>141</v>
@@ -2485,7 +2479,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="12" t="s">
         <v>142</v>
@@ -2494,7 +2488,7 @@
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="13" t="s">
         <v>143</v>
@@ -2503,7 +2497,7 @@
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="12" t="s">
         <v>144</v>
@@ -2512,7 +2506,7 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="10" t="s">
         <v>77</v>
@@ -2521,7 +2515,7 @@
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="11" t="s">
         <v>78</v>
@@ -2530,7 +2524,7 @@
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="10" t="s">
         <v>79</v>
@@ -2539,7 +2533,7 @@
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="11" t="s">
         <v>80</v>
@@ -2548,7 +2542,7 @@
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="10" t="s">
         <v>81</v>
@@ -2557,7 +2551,7 @@
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="11" t="s">
         <v>82</v>
@@ -2566,7 +2560,7 @@
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="10" t="s">
         <v>83</v>
@@ -2575,7 +2569,7 @@
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="11" t="s">
         <v>84</v>
@@ -2584,7 +2578,7 @@
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="10" t="s">
         <v>85</v>
@@ -2593,7 +2587,7 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="11" t="s">
         <v>86</v>
@@ -2602,7 +2596,7 @@
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="13" t="s">
         <v>145</v>
@@ -2611,7 +2605,7 @@
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="12" t="s">
         <v>146</v>
@@ -2620,7 +2614,7 @@
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="13" t="s">
         <v>147</v>
@@ -2629,7 +2623,7 @@
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="12" t="s">
         <v>148</v>
@@ -2638,7 +2632,7 @@
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="13" t="s">
         <v>149</v>
@@ -2647,7 +2641,7 @@
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="11" t="s">
         <v>87</v>
@@ -2656,7 +2650,7 @@
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="10" t="s">
         <v>88</v>
@@ -2665,7 +2659,7 @@
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="11" t="s">
         <v>89</v>
@@ -2674,7 +2668,7 @@
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="10" t="s">
         <v>90</v>
@@ -2683,7 +2677,7 @@
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="11" t="s">
         <v>91</v>
@@ -2692,7 +2686,7 @@
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="10" t="s">
         <v>92</v>
@@ -2701,7 +2695,7 @@
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="11" t="s">
         <v>93</v>
@@ -2710,7 +2704,7 @@
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="10" t="s">
         <v>94</v>
@@ -2719,7 +2713,7 @@
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="11" t="s">
         <v>95</v>
@@ -2728,7 +2722,7 @@
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="10" t="s">
         <v>96</v>
@@ -2737,7 +2731,7 @@
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="11" t="s">
         <v>97</v>
@@ -2746,7 +2740,7 @@
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="10" t="s">
         <v>98</v>
@@ -2755,7 +2749,7 @@
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="11" t="s">
         <v>99</v>
@@ -2764,7 +2758,7 @@
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="10" t="s">
         <v>100</v>
@@ -2773,7 +2767,7 @@
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="11" t="s">
         <v>101</v>
@@ -2782,7 +2776,7 @@
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="10" t="s">
         <v>102</v>
@@ -2791,7 +2785,7 @@
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="11" t="s">
         <v>103</v>
@@ -2800,7 +2794,7 @@
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="10" t="s">
         <v>104</v>
@@ -2809,7 +2803,7 @@
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="11" t="s">
         <v>105</v>
@@ -2818,7 +2812,7 @@
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="10" t="s">
         <v>106</v>
@@ -2827,7 +2821,7 @@
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="11" t="s">
         <v>107</v>
@@ -2836,7 +2830,7 @@
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="10" t="s">
         <v>108</v>
@@ -2845,7 +2839,7 @@
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="11" t="s">
         <v>109</v>
@@ -2854,7 +2848,7 @@
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="10" t="s">
         <v>110</v>
@@ -2863,7 +2857,7 @@
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="11" t="s">
         <v>111</v>
@@ -2872,7 +2866,7 @@
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="B100" s="13" t="s">
         <v>150</v>
@@ -2881,7 +2875,7 @@
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="12" t="s">
         <v>151</v>
@@ -2890,7 +2884,7 @@
       <c r="D101" s="6"/>
       <c r="E101" s="6"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
       <c r="B102" s="10" t="s">
         <v>112</v>
@@ -2899,7 +2893,7 @@
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="11" t="s">
         <v>113</v>
@@ -2908,7 +2902,7 @@
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="10" t="s">
         <v>114</v>
@@ -2917,7 +2911,7 @@
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="11" t="s">
         <v>115</v>
@@ -2926,7 +2920,7 @@
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
       <c r="B106" s="10" t="s">
         <v>116</v>
@@ -2935,7 +2929,7 @@
       <c r="D106" s="6"/>
       <c r="E106" s="6"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="11" t="s">
         <v>117</v>
@@ -2944,7 +2938,7 @@
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="13" t="s">
         <v>152</v>
@@ -2953,7 +2947,7 @@
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="11" t="s">
         <v>118</v>
@@ -2962,7 +2956,7 @@
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
       <c r="B110" s="10" t="s">
         <v>119</v>
@@ -2971,7 +2965,7 @@
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
       <c r="B111" s="9" t="s">
         <v>120</v>
@@ -2990,15 +2984,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003082C08FD3D0614AAB94B75C024070A7" ma:contentTypeVersion="29" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a4b61487ffa532d49c6719891dd0d2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="82302deb-32b0-442b-bedc-ba64a9aa8ccd" xmlns:ns3="cc7ce8ca-8f52-44ec-9496-3c41d0f5ad18" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cea40d1c5f6ee0e5ae997cf8704aff88" ns2:_="" ns3:_="">
     <xsd:import namespace="82302deb-32b0-442b-bedc-ba64a9aa8ccd"/>
@@ -3287,6 +3272,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3306,14 +3300,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{675DE784-F3DF-4BF9-9432-B8FB7941C39F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B39BBA2A-0161-425D-935A-F961630DCAA3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3328,6 +3314,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{675DE784-F3DF-4BF9-9432-B8FB7941C39F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>